<commit_message>
Merged PR 21: mergeback
Related work items: #250, #251
</commit_message>
<xml_diff>
--- a/DesignerRawdata/Excel/Test.xlsx
+++ b/DesignerRawdata/Excel/Test.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FF05FD-7070-4F25-AB1A-D5352A87FCF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEF49CA-7A31-4A2A-963B-E404DDB9AAB4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,9 +92,56 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;text color="#77FF77AA" shadowColor="#FF0000FF" shadowOffset="[4,3]"&gt;This is rich text simple test:&lt;/text&gt;&lt;br/&gt;
+    <t xml:space="preserve">&lt;text color="#77FF77AA" shadowColor="#FF0000FF" shadowOffset="[4,3]"&gt;This is rich text simple test:&lt;/text&gt;&lt;br/&gt;
 &lt;text color="#FF0000AA"&gt;This is programmer:&lt;/text&gt;&lt;img filePath="PaperSprite'/Game/HorizonUIDemo/SpriteSheet/Test/Frames/programmer_png.programmer_png'" size="[50, 50]" /&gt;&lt;br/&gt;
-&lt;text color="#0000FFFF"&gt;This is a WaterMellon:&lt;/text&gt;&lt;img color="#FF00FF77" filePath="PaperSprite'/Game/HorizonUIDemo/SpriteSheet/Test/Frames/I_C_Watermellon_png.I_C_Watermellon_png'" size="[25, 25]" /&gt; &lt;br/&gt;</t>
+&lt;text color="#0000FFFF"&gt;This is a WaterMellon:&lt;/text&gt;&lt;img color="#FF00FF77" filePath="PaperSprite'/Game/HorizonUIDemo/SpriteSheet/Test/Frames/I_C_Watermellon_png.I_C_Watermellon_png'" size="[50, 50]" /&gt; &lt;br/&gt;
+&lt;text color="#77FF77AA" shadowColor="#FF0000FF" shadowOffset="[4,3]"&gt;This is rich text simple test:&lt;/text&gt;&lt;br/&gt;
+&lt;text&gt;Test Message 1234578910111213141516171819&lt;/text&gt;&lt;br/&gt;
+&lt;text color="#77FF77AA" shadowColor="#FF0000FF" shadowOffset="[4,3]"&gt;This is rich text simple test:&lt;/text&gt;&lt;br/&gt;
+&lt;text color="#FF0000AA"&gt;This is strawberry:&lt;/text&gt;&lt;img filePath="Texture2D'/Game/HorizonUIDemo/Texture/Item/I_C_Strawberry.I_C_Strawberry'" size="[50, 50]" /&gt;&lt;br/&gt;
+&lt;text color="#0000FFFF"&gt;This is Watermellon:&lt;/text&gt;&lt;img color="#FF00FF77" filePath="Texture2D'/Game/HorizonUIDemo/Texture/Item/I_C_Watermellon.I_C_Watermellon'" size="[50, 50]" /&gt; &lt;br/&gt;
+&lt;text color="#FFFF00FF"&gt;This is animated man using material:&lt;/text&gt;&lt;img filePath="Material'/Game/HorizonUIDemo/Material/mat_flipbook.mat_flipbook'" size="[50, 50]" /&gt; &lt;br/&gt;
+&lt;text&gt;This is Default Font&lt;/text&gt;&lt;br/&gt;
+&lt;text fontPath="/Engine/EngineFonts/Roboto" fontType="Regular" fontSize="30"&gt;This is Roboto Regular fontSize=30&lt;/text&gt;&lt;br/&gt;
+&lt;text fontPath="/Engine/EngineFonts/Roboto" fontType="Italic" color="#FF0000AA"&gt;This is Roboto Italic&lt;/text&gt;&lt;br/&gt;
+&lt;text fontPath="/Engine/EngineFonts/Roboto" fontType="Bold Italic"  fontSize="40" color="#FF3366AA"&gt;This is Roboto Bold Italic fontSize=40&lt;/text&gt;&lt;br/&gt;
+&lt;text fontPath="/Engine/EngineFonts/Roboto" fontType="Light" color="#FFFF00AA"&gt;This is Roboto Light&lt;/text&gt;&lt;br/&gt;
+&lt;text fontPath="/Engine/EngineFonts/RobotoTiny" fontType="Light" color="#FF0A40AA"&gt;This is RobotoTinyLight&lt;/text&gt;&lt;br/&gt;
+&lt;text fontSize="25"&gt;Test case:&lt;/text&gt; 
+&lt;text padding-right="5" padding-top="20"&gt;
+ &lt;text padding-left="5"&gt;padding text block&lt;/text&gt;
+ &lt;img filePath="Material'/Game/HorizonUIDemo/Material/mat_flipbook.mat_flipbook'"/&gt;
+ &lt;img filePath="Texture2D'/Game/HorizonUIDemo/Texture/Item/I_C_Watermellon.I_C_Watermellon'" size="[50,50]" /&gt;
+&lt;/text&gt;&lt;br/&gt;
+&lt;text&gt;after padding&lt;/text&gt;&lt;br/&gt;&lt;br/&gt;
+&lt;text color="#77FF77AA" shadowColor="#FF0000FF" shadowOffset="[4,3]" &gt; color, shadow color and offset &lt;/text&gt;&lt;br/&gt;&lt;br/&gt;
+&lt;text&gt; 
+&lt;text color="#FF0000FF"&gt; Nested  &lt;/text&gt;
+&lt;text color="#FF00FFFF"&gt;
+&amp;nbsp;tag node 
+&lt;/text&gt;&lt;br/&gt;
+&lt;text color="#FFFF00FF"&gt;
+ &amp;nbsp;Dialogue Text 
+&lt;/text&gt;&lt;br/&gt;
+&lt;text color="#FF0000FF"&gt;
+&amp;nbsp;Block  
+&lt;/text&gt;&lt;br/&gt;
+&lt;/text&gt;
+&lt;a href="Seg1ClickMessage" bgColor="#555555FF" hoverColor="#FFFF0055" filePath="Blueprint'/Game/HorizonUIDemo/ButtonStyle/BP_DialogueBackgroundButtonStyle1.BP_DialogueBackgroundButtonStyle1'"&gt;
+&lt;text color="#FF0000FF"&gt; Test Click Seg1  &lt;/text&gt;
+&lt;/a&gt;&lt;br/&gt;
+&lt;a href="Seg2ClickMessage" bgColor="#FF0000FF" hoverColor="#FFFF0055" filePath="Blueprint'/Game/HorizonUIDemo/ButtonStyle/BP_DialogueBackgroundButtonStyle2.BP_DialogueBackgroundButtonStyle2'"&gt;
+&lt;text color="#00FF00FF"&gt; Test Click Seg2  &lt;/text&gt;
+&lt;/a&gt;&lt;br/&gt;
+&lt;a href="Seg3ClickMessage" bgColor="#FF0000FF" hoverColor="#FFFF0055" filePath="Blueprint'/Game/HorizonUIDemo/ButtonStyle/BP_DialogueBackgroundButtonStyle3.BP_DialogueBackgroundButtonStyle3'"&gt;
+&lt;text color="#0000FFFF"&gt; Test Click Seg3  &lt;/text&gt;
+&lt;/a&gt;&lt;br/&gt;
+&lt;text style="bp1.style1"&gt;This is rich text test using style:&lt;/text&gt;&lt;br/&gt;
+&lt;text style="bp1.style2"&gt;This is strawberry:&lt;/text&gt;&lt;img style="bp1.style1" /&gt;&lt;br/&gt;
+&lt;text style="bp2.style1"&gt;This is Watermellon:&lt;/text&gt;&lt;img style="bp2.style1"/&gt; &lt;br/&gt;
+&lt;text style="bp2.style2"&gt;This is animated man using material:&lt;/text&gt;&lt;mat style="bp2.style2" /&gt; &lt;br/&gt;
+&lt;text style="bp2.style3"&gt;Horizon Flipbook Widget (use tag pfb) Only Supported by using style:&lt;/text&gt;&lt;pfb style="bp2.style1" /&gt; &lt;br/&gt;
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -174,6 +221,31 @@
         <row r="2">
           <cell r="A2" t="str">
             <v>id_programmer</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>id_designer</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>id_artist</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>id_unknwon</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>id_test</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>id_test2</v>
           </cell>
         </row>
       </sheetData>
@@ -447,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -531,7 +603,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Merged PR 22: Dialogue FunctionTest
Related work items: #250, #252, #253, #254, #255, #256, #257, #258, #259, #262, #348
</commit_message>
<xml_diff>
--- a/DesignerRawdata/Excel/Test.xlsx
+++ b/DesignerRawdata/Excel/Test.xlsx
@@ -3,15 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEEF49CA-7A31-4A2A-963B-E404DDB9AAB4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070187E7-67A5-48FB-9081-59411BEA1EB1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test_Title" sheetId="2" r:id="rId1"/>
+    <sheet name="Test_Content" sheetId="1" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="DialogueTalkerName.xlsx">[1]!DialogueTalkerNameID</definedName>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>id_001</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -142,6 +143,13 @@
 &lt;text style="bp2.style2"&gt;This is animated man using material:&lt;/text&gt;&lt;mat style="bp2.style2" /&gt; &lt;br/&gt;
 &lt;text style="bp2.style3"&gt;Horizon Flipbook Widget (use tag pfb) Only Supported by using style:&lt;/text&gt;&lt;pfb style="bp2.style1" /&gt; &lt;br/&gt;
 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id_test</t>
+  </si>
+  <si>
+    <t>Long Dialogue Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -516,18 +524,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D944F81E-5369-42AC-AE8C-300297A3D42E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A1" xr:uid="{1E7EC4AB-D541-4165-B09A-CF782ABF7DCD}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="160.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="92.85546875" customWidth="1"/>
     <col min="4" max="4" width="62.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -543,6 +591,9 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
@@ -551,6 +602,9 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -559,6 +613,9 @@
       <c r="A4" t="s">
         <v>17</v>
       </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -567,6 +624,9 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
@@ -575,6 +635,9 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
@@ -583,6 +646,9 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
@@ -591,6 +657,9 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
@@ -599,6 +668,9 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>
@@ -606,6 +678,9 @@
     <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>19</v>

</xml_diff>